<commit_message>
final de cuartos de final
</commit_message>
<xml_diff>
--- a/Copa America 2016.xlsx
+++ b/Copa America 2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="30" windowWidth="9510" windowHeight="4710" tabRatio="542" activeTab="2"/>
+    <workbookView xWindow="12090" yWindow="30" windowWidth="9510" windowHeight="4710" tabRatio="542" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Grupos" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -277,27 +277,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -322,15 +303,41 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color indexed="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="28"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="28"/>
-      <color indexed="10"/>
+      <sz val="18"/>
+      <color indexed="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -943,7 +950,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1067,13 +1074,13 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1106,58 +1113,58 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1166,34 +1173,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1205,37 +1212,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3659,7 +3666,7 @@
   <dimension ref="B1:T22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3705,7 +3712,7 @@
     </row>
     <row r="2" spans="2:20" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K2" s="131" t="str">
-        <f>IF(E17&gt;H17,C17,F17)</f>
+        <f>IF(E17&gt;H17,C17,IF(E17&lt;H17,F17,""))</f>
         <v/>
       </c>
       <c r="L2" s="132"/>
@@ -3890,15 +3897,19 @@
         <v>EE. UU.</v>
       </c>
       <c r="D10" s="119"/>
-      <c r="E10" s="41"/>
+      <c r="E10" s="41">
+        <v>0</v>
+      </c>
       <c r="F10" s="119" t="str">
-        <f>IF(E5&gt;H5,D5,IF(E5&lt;H5,G5,""))</f>
-        <v>Colombia</v>
+        <f>IF(E6&gt;H6,D6,IF(E6&lt;H6,G6,""))</f>
+        <v>Argentina</v>
       </c>
       <c r="G10" s="119"/>
-      <c r="H10" s="65"/>
+      <c r="H10" s="65">
+        <v>4</v>
+      </c>
       <c r="K10" s="99" t="str">
-        <f>IF(E17&gt;H17,C17,F17)</f>
+        <f>IF(E17&gt;H17,C17,IF(E17&lt;H17,F17,""))</f>
         <v/>
       </c>
       <c r="L10" s="100"/>
@@ -3913,17 +3924,21 @@
     <row r="11" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="97"/>
       <c r="C11" s="127" t="str">
-        <f>IF(E6&gt;H6,D6,IF(E6&lt;H6,G6,""))</f>
-        <v>Argentina</v>
+        <f>IF(E5&gt;H5,D5,IF(E5&lt;H5,G5,""))</f>
+        <v>Colombia</v>
       </c>
       <c r="D11" s="128"/>
-      <c r="E11" s="48"/>
+      <c r="E11" s="48">
+        <v>0</v>
+      </c>
       <c r="F11" s="128" t="str">
         <f>IF(E7&gt;H7,D7,IF(E7&lt;H7,G7,""))</f>
         <v>Chile</v>
       </c>
       <c r="G11" s="128"/>
-      <c r="H11" s="67"/>
+      <c r="H11" s="67">
+        <v>2</v>
+      </c>
       <c r="K11" s="102"/>
       <c r="L11" s="103"/>
       <c r="M11" s="103"/>
@@ -3966,13 +3981,13 @@
       <c r="B14" s="130"/>
       <c r="C14" s="114" t="str">
         <f>IF(E10&lt;H10,C10,IF(E10&gt;H10,F10,""))</f>
-        <v/>
+        <v>EE. UU.</v>
       </c>
       <c r="D14" s="115"/>
       <c r="E14" s="50"/>
       <c r="F14" s="115" t="str">
         <f>IF(E11&lt;H11,C11,IF(E11&gt;H11,F11,""))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="G14" s="115"/>
       <c r="H14" s="68"/>
@@ -3986,7 +4001,7 @@
     </row>
     <row r="15" spans="2:20" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K15" s="99" t="str">
-        <f>IF(E14&gt;H14,C14,F14)</f>
+        <f>IF(E14&gt;H14,C14,IF(E14&lt;H14,F14,""))</f>
         <v/>
       </c>
       <c r="L15" s="100"/>
@@ -4024,13 +4039,13 @@
       <c r="B17" s="97"/>
       <c r="C17" s="114" t="str">
         <f>IF(E10&gt;H10,C10,IF(E10&lt;H10,F10,""))</f>
-        <v/>
+        <v>Argentina</v>
       </c>
       <c r="D17" s="115"/>
       <c r="E17" s="50"/>
       <c r="F17" s="115" t="str">
         <f>IF(E11&gt;H11,C11,IF(E11&lt;H11,F11,""))</f>
-        <v/>
+        <v>Chile</v>
       </c>
       <c r="G17" s="115"/>
       <c r="H17" s="68"/>

</xml_diff>

<commit_message>
termino la copa america
</commit_message>
<xml_diff>
--- a/Copa America 2016.xlsx
+++ b/Copa America 2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="30" windowWidth="9510" windowHeight="4710" tabRatio="542" activeTab="2"/>
+    <workbookView xWindow="14880" yWindow="30" windowWidth="9510" windowHeight="4710" tabRatio="542" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Grupos" sheetId="1" r:id="rId1"/>
@@ -283,13 +283,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="72"/>
-      <color indexed="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -341,6 +334,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -866,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1047,6 +1047,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1065,6 +1068,36 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1074,175 +1107,136 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1851,26 +1845,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
     </row>
     <row r="4" spans="2:9" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="62" t="s">
@@ -1989,54 +1983,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="H1" s="81" t="s">
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="H1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="82"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="93"/>
     </row>
     <row r="2" spans="1:25" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="85"/>
-      <c r="H2" s="80" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="96"/>
+      <c r="H2" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
     </row>
     <row r="4" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="51"/>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
       <c r="I4" s="7" t="s">
         <v>14</v>
       </c>
@@ -2087,7 +2081,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="81" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="13" t="str">
@@ -2105,7 +2099,7 @@
       <c r="F5" s="28">
         <v>2</v>
       </c>
-      <c r="H5" s="88" t="s">
+      <c r="H5" s="81" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="53" t="str">
@@ -2166,7 +2160,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="89"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="11" t="str">
         <f>Grupos!B7</f>
         <v>Costa Rica</v>
@@ -2182,7 +2176,7 @@
       <c r="F6" s="29">
         <v>0</v>
       </c>
-      <c r="H6" s="89"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="56" t="str">
         <f>Grupos!B6</f>
         <v>Colombia</v>
@@ -2241,7 +2235,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="89"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="11" t="str">
         <f>Grupos!B5</f>
         <v>EE. UU.</v>
@@ -2257,7 +2251,7 @@
       <c r="F7" s="29">
         <v>0</v>
       </c>
-      <c r="H7" s="89"/>
+      <c r="H7" s="82"/>
       <c r="I7" s="56" t="str">
         <f>Grupos!B7</f>
         <v>Costa Rica</v>
@@ -2316,7 +2310,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="89"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="11" t="str">
         <f>Grupos!B6</f>
         <v>Colombia</v>
@@ -2332,7 +2326,7 @@
       <c r="F8" s="29">
         <v>1</v>
       </c>
-      <c r="H8" s="90"/>
+      <c r="H8" s="83"/>
       <c r="I8" s="59" t="str">
         <f>Grupos!B8</f>
         <v>Paraguay</v>
@@ -2391,7 +2385,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="89"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="11" t="str">
         <f>Grupos!B5</f>
         <v>EE. UU.</v>
@@ -2409,7 +2403,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="90"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="15" t="str">
         <f>Grupos!B6</f>
         <v>Colombia</v>
@@ -2432,13 +2426,13 @@
     </row>
     <row r="11" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
       <c r="I12" s="7" t="s">
         <v>14</v>
       </c>
@@ -2489,7 +2483,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="81" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="17" t="str">
@@ -2507,7 +2501,7 @@
       <c r="F13" s="34">
         <v>0</v>
       </c>
-      <c r="H13" s="88" t="s">
+      <c r="H13" s="81" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="53" t="str">
@@ -2568,7 +2562,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="91"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="20" t="str">
         <f>Grupos!D7</f>
         <v>Haiti</v>
@@ -2584,7 +2578,7 @@
       <c r="F14" s="35">
         <v>1</v>
       </c>
-      <c r="H14" s="89"/>
+      <c r="H14" s="82"/>
       <c r="I14" s="56" t="str">
         <f>Grupos!D6</f>
         <v>Ecuador</v>
@@ -2643,7 +2637,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="91"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="20" t="str">
         <f>Grupos!D5</f>
         <v>Brasil</v>
@@ -2659,7 +2653,7 @@
       <c r="F15" s="35">
         <v>1</v>
       </c>
-      <c r="H15" s="89"/>
+      <c r="H15" s="82"/>
       <c r="I15" s="56" t="str">
         <f>Grupos!D7</f>
         <v>Haiti</v>
@@ -2718,7 +2712,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="91"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="20" t="str">
         <f>Grupos!D6</f>
         <v>Ecuador</v>
@@ -2734,7 +2728,7 @@
       <c r="F16" s="35">
         <v>2</v>
       </c>
-      <c r="H16" s="90"/>
+      <c r="H16" s="83"/>
       <c r="I16" s="59" t="str">
         <f>Grupos!D8</f>
         <v>Perú</v>
@@ -2793,7 +2787,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="91"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="20" t="str">
         <f>Grupos!D5</f>
         <v>Brasil</v>
@@ -2811,7 +2805,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="92"/>
+      <c r="A18" s="85"/>
       <c r="B18" s="19" t="str">
         <f>Grupos!D6</f>
         <v>Ecuador</v>
@@ -2830,13 +2824,13 @@
     </row>
     <row r="19" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
       <c r="I20" s="7" t="s">
         <v>14</v>
       </c>
@@ -2887,7 +2881,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="86" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="22" t="str">
@@ -2905,7 +2899,7 @@
       <c r="F21" s="34">
         <v>1</v>
       </c>
-      <c r="H21" s="88" t="s">
+      <c r="H21" s="81" t="s">
         <v>21</v>
       </c>
       <c r="I21" s="53" t="str">
@@ -2966,7 +2960,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="94"/>
+      <c r="A22" s="87"/>
       <c r="B22" s="24" t="str">
         <f>Grupos!F7</f>
         <v>Jamaica</v>
@@ -2982,7 +2976,7 @@
       <c r="F22" s="35">
         <v>1</v>
       </c>
-      <c r="H22" s="89"/>
+      <c r="H22" s="82"/>
       <c r="I22" s="56" t="str">
         <f>Grupos!F6</f>
         <v>Uruguay</v>
@@ -3041,7 +3035,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="94"/>
+      <c r="A23" s="87"/>
       <c r="B23" s="24" t="str">
         <f>Grupos!F5</f>
         <v>Mexico</v>
@@ -3057,7 +3051,7 @@
       <c r="F23" s="35">
         <v>0</v>
       </c>
-      <c r="H23" s="89"/>
+      <c r="H23" s="82"/>
       <c r="I23" s="56" t="str">
         <f>Grupos!F7</f>
         <v>Jamaica</v>
@@ -3116,7 +3110,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="94"/>
+      <c r="A24" s="87"/>
       <c r="B24" s="24" t="str">
         <f>Grupos!F6</f>
         <v>Uruguay</v>
@@ -3132,7 +3126,7 @@
       <c r="F24" s="35">
         <v>1</v>
       </c>
-      <c r="H24" s="90"/>
+      <c r="H24" s="83"/>
       <c r="I24" s="59" t="str">
         <f>Grupos!F8</f>
         <v>Venezuela</v>
@@ -3191,7 +3185,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="94"/>
+      <c r="A25" s="87"/>
       <c r="B25" s="24" t="str">
         <f>Grupos!F5</f>
         <v>Mexico</v>
@@ -3209,7 +3203,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="95"/>
+      <c r="A26" s="88"/>
       <c r="B26" s="23" t="str">
         <f>Grupos!F6</f>
         <v>Uruguay</v>
@@ -3228,13 +3222,13 @@
     </row>
     <row r="27" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="86" t="s">
+      <c r="B28" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
       <c r="I28" s="7" t="s">
         <v>14</v>
       </c>
@@ -3285,7 +3279,7 @@
       </c>
     </row>
     <row r="29" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="86" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="22" t="str">
@@ -3303,7 +3297,7 @@
       <c r="F29" s="34">
         <v>1</v>
       </c>
-      <c r="H29" s="88" t="s">
+      <c r="H29" s="81" t="s">
         <v>23</v>
       </c>
       <c r="I29" s="53" t="str">
@@ -3364,7 +3358,7 @@
       </c>
     </row>
     <row r="30" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="94"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="24" t="str">
         <f>Grupos!H7</f>
         <v>Panamá</v>
@@ -3380,7 +3374,7 @@
       <c r="F30" s="35">
         <v>1</v>
       </c>
-      <c r="H30" s="89"/>
+      <c r="H30" s="82"/>
       <c r="I30" s="56" t="str">
         <f>Grupos!H6</f>
         <v>Chile</v>
@@ -3439,7 +3433,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="94"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="24" t="str">
         <f>Grupos!H5</f>
         <v>Argentina</v>
@@ -3455,7 +3449,7 @@
       <c r="F31" s="35">
         <v>0</v>
       </c>
-      <c r="H31" s="89"/>
+      <c r="H31" s="82"/>
       <c r="I31" s="56" t="str">
         <f>Grupos!H7</f>
         <v>Panamá</v>
@@ -3514,7 +3508,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="94"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="24" t="str">
         <f>Grupos!H6</f>
         <v>Chile</v>
@@ -3530,7 +3524,7 @@
       <c r="F32" s="35">
         <v>1</v>
       </c>
-      <c r="H32" s="90"/>
+      <c r="H32" s="83"/>
       <c r="I32" s="59" t="str">
         <f>Grupos!H8</f>
         <v>Bolivia</v>
@@ -3589,7 +3583,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="94"/>
+      <c r="A33" s="87"/>
       <c r="B33" s="24" t="str">
         <f>Grupos!H5</f>
         <v>Argentina</v>
@@ -3607,7 +3601,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="95"/>
+      <c r="A34" s="88"/>
       <c r="B34" s="23" t="str">
         <f>Grupos!H6</f>
         <v>Chile</v>
@@ -3627,6 +3621,12 @@
     <row r="35" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:P2"/>
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A21:A26"/>
@@ -3637,12 +3637,6 @@
     <mergeCell ref="H29:H32"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="B20:F20"/>
-    <mergeCell ref="H2:P2"/>
-    <mergeCell ref="H1:P1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3666,7 +3660,7 @@
   <dimension ref="B1:T22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3691,59 +3685,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="125"/>
-      <c r="K1" s="116" t="s">
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="108"/>
+      <c r="K1" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="118"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="2:20" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="131" t="str">
+      <c r="K2" s="129" t="str">
         <f>IF(E17&gt;H17,C17,IF(E17&lt;H17,F17,""))</f>
-        <v/>
-      </c>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132"/>
-      <c r="O2" s="132"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="133"/>
+        <v>Chile</v>
+      </c>
+      <c r="L2" s="130"/>
+      <c r="M2" s="130"/>
+      <c r="N2" s="130"/>
+      <c r="O2" s="130"/>
+      <c r="P2" s="130"/>
+      <c r="Q2" s="131"/>
     </row>
     <row r="3" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="122"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="136"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="105"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="133"/>
+      <c r="Q3" s="134"/>
     </row>
     <row r="4" spans="2:20" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="98"/>
+      <c r="B4" s="110"/>
       <c r="C4" s="44" t="s">
         <v>31</v>
       </c>
@@ -3764,17 +3758,17 @@
       <c r="H4" s="65">
         <v>1</v>
       </c>
-      <c r="K4" s="134"/>
-      <c r="L4" s="135"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="135"/>
-      <c r="Q4" s="136"/>
+      <c r="K4" s="132"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="133"/>
+      <c r="Q4" s="134"/>
       <c r="T4" s="37"/>
     </row>
-    <row r="5" spans="2:20" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="98"/>
+    <row r="5" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="110"/>
       <c r="C5" s="45" t="s">
         <v>29</v>
       </c>
@@ -3795,16 +3789,16 @@
       <c r="H5" s="66">
         <v>4</v>
       </c>
-      <c r="K5" s="134"/>
-      <c r="L5" s="135"/>
-      <c r="M5" s="135"/>
-      <c r="N5" s="135"/>
-      <c r="O5" s="135"/>
-      <c r="P5" s="135"/>
-      <c r="Q5" s="136"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="136"/>
+      <c r="N5" s="136"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
+      <c r="Q5" s="137"/>
     </row>
     <row r="6" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="98"/>
+      <c r="B6" s="110"/>
       <c r="C6" s="45" t="s">
         <v>30</v>
       </c>
@@ -3825,17 +3819,17 @@
       <c r="H6" s="66">
         <v>1</v>
       </c>
-      <c r="K6" s="137"/>
-      <c r="L6" s="138"/>
-      <c r="M6" s="138"/>
-      <c r="N6" s="138"/>
-      <c r="O6" s="138"/>
-      <c r="P6" s="138"/>
-      <c r="Q6" s="139"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
       <c r="T6" s="37"/>
     </row>
     <row r="7" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="97"/>
+      <c r="B7" s="111"/>
       <c r="C7" s="46" t="s">
         <v>32</v>
       </c>
@@ -3856,96 +3850,103 @@
       <c r="H7" s="67">
         <v>7</v>
       </c>
+      <c r="K7" s="97" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="99"/>
     </row>
     <row r="8" spans="2:20" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K8" s="105" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="107"/>
+      <c r="K8" s="117"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="118"/>
+      <c r="Q8" s="119"/>
     </row>
     <row r="9" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="120" t="s">
+      <c r="C9" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="121"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="121"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="122"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
-      <c r="O9" s="109"/>
-      <c r="P9" s="109"/>
-      <c r="Q9" s="110"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="105"/>
+      <c r="K9" s="120" t="str">
+        <f>IF(E17&gt;H17,F17,IF(E17&lt;H17,C17,""))</f>
+        <v>Argentina</v>
+      </c>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="122"/>
       <c r="R9" s="37"/>
       <c r="S9" s="37"/>
     </row>
     <row r="10" spans="2:20" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="98"/>
-      <c r="C10" s="126" t="str">
+      <c r="B10" s="110"/>
+      <c r="C10" s="112" t="str">
         <f>IF(E4&gt;H4,D4,IF(E4&lt;H4,G4,""))</f>
         <v>EE. UU.</v>
       </c>
-      <c r="D10" s="119"/>
+      <c r="D10" s="102"/>
       <c r="E10" s="41">
         <v>0</v>
       </c>
-      <c r="F10" s="119" t="str">
+      <c r="F10" s="102" t="str">
         <f>IF(E6&gt;H6,D6,IF(E6&lt;H6,G6,""))</f>
         <v>Argentina</v>
       </c>
-      <c r="G10" s="119"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="65">
         <v>4</v>
       </c>
-      <c r="K10" s="99" t="str">
-        <f>IF(E17&gt;H17,C17,IF(E17&lt;H17,F17,""))</f>
-        <v/>
-      </c>
-      <c r="L10" s="100"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="100"/>
-      <c r="O10" s="100"/>
-      <c r="P10" s="100"/>
-      <c r="Q10" s="101"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="124"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="124"/>
+      <c r="O10" s="124"/>
+      <c r="P10" s="124"/>
+      <c r="Q10" s="125"/>
       <c r="R10" s="37"/>
       <c r="S10" s="37"/>
     </row>
     <row r="11" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="97"/>
-      <c r="C11" s="127" t="str">
+      <c r="B11" s="111"/>
+      <c r="C11" s="113" t="str">
         <f>IF(E5&gt;H5,D5,IF(E5&lt;H5,G5,""))</f>
         <v>Colombia</v>
       </c>
-      <c r="D11" s="128"/>
+      <c r="D11" s="114"/>
       <c r="E11" s="48">
         <v>0</v>
       </c>
-      <c r="F11" s="128" t="str">
+      <c r="F11" s="114" t="str">
         <f>IF(E7&gt;H7,D7,IF(E7&lt;H7,G7,""))</f>
         <v>Chile</v>
       </c>
-      <c r="G11" s="128"/>
+      <c r="G11" s="114"/>
       <c r="H11" s="67">
         <v>2</v>
       </c>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="104"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="127"/>
+      <c r="M11" s="127"/>
+      <c r="N11" s="127"/>
+      <c r="O11" s="127"/>
+      <c r="P11" s="127"/>
+      <c r="Q11" s="128"/>
       <c r="R11" s="37"/>
       <c r="S11" s="37"/>
     </row>
@@ -3954,108 +3955,116 @@
       <c r="S12" s="37"/>
     </row>
     <row r="13" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="129" t="s">
+      <c r="B13" s="115" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="120" t="s">
+      <c r="C13" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="121"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
-      <c r="H13" s="122"/>
-      <c r="K13" s="105" t="s">
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="105"/>
+      <c r="K13" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="106"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="107"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="99"/>
       <c r="R13" s="37"/>
       <c r="S13" s="37"/>
     </row>
     <row r="14" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="130"/>
-      <c r="C14" s="114" t="str">
+      <c r="B14" s="116"/>
+      <c r="C14" s="100" t="str">
         <f>IF(E10&lt;H10,C10,IF(E10&gt;H10,F10,""))</f>
         <v>EE. UU.</v>
       </c>
-      <c r="D14" s="115"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="115" t="str">
+      <c r="D14" s="101"/>
+      <c r="E14" s="50">
+        <v>0</v>
+      </c>
+      <c r="F14" s="101" t="str">
         <f>IF(E11&lt;H11,C11,IF(E11&gt;H11,F11,""))</f>
         <v>Colombia</v>
       </c>
-      <c r="G14" s="115"/>
-      <c r="H14" s="68"/>
-      <c r="K14" s="108"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="109"/>
-      <c r="N14" s="109"/>
-      <c r="O14" s="109"/>
-      <c r="P14" s="109"/>
-      <c r="Q14" s="110"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="68">
+        <v>1</v>
+      </c>
+      <c r="K14" s="117"/>
+      <c r="L14" s="118"/>
+      <c r="M14" s="118"/>
+      <c r="N14" s="118"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="118"/>
+      <c r="Q14" s="119"/>
     </row>
     <row r="15" spans="2:20" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K15" s="99" t="str">
+      <c r="K15" s="120" t="str">
         <f>IF(E14&gt;H14,C14,IF(E14&lt;H14,F14,""))</f>
-        <v/>
-      </c>
-      <c r="L15" s="100"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="100"/>
-      <c r="O15" s="100"/>
-      <c r="P15" s="100"/>
-      <c r="Q15" s="101"/>
+        <v>Colombia</v>
+      </c>
+      <c r="L15" s="121"/>
+      <c r="M15" s="121"/>
+      <c r="N15" s="121"/>
+      <c r="O15" s="121"/>
+      <c r="P15" s="121"/>
+      <c r="Q15" s="122"/>
       <c r="R15" s="37"/>
       <c r="S15" s="37"/>
     </row>
     <row r="16" spans="2:20" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="121"/>
-      <c r="E16" s="121"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="121"/>
-      <c r="H16" s="122"/>
-      <c r="K16" s="111"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
-      <c r="N16" s="112"/>
-      <c r="O16" s="112"/>
-      <c r="P16" s="112"/>
-      <c r="Q16" s="113"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="104"/>
+      <c r="H16" s="105"/>
+      <c r="K16" s="123"/>
+      <c r="L16" s="124"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="124"/>
+      <c r="P16" s="124"/>
+      <c r="Q16" s="125"/>
       <c r="R16" s="37"/>
       <c r="S16" s="37"/>
     </row>
     <row r="17" spans="2:17" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="97"/>
-      <c r="C17" s="114" t="str">
+      <c r="B17" s="111"/>
+      <c r="C17" s="100" t="str">
         <f>IF(E10&gt;H10,C10,IF(E10&lt;H10,F10,""))</f>
         <v>Argentina</v>
       </c>
-      <c r="D17" s="115"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="115" t="str">
+      <c r="D17" s="101"/>
+      <c r="E17" s="50">
+        <v>2</v>
+      </c>
+      <c r="F17" s="101" t="str">
         <f>IF(E11&gt;H11,C11,IF(E11&lt;H11,F11,""))</f>
         <v>Chile</v>
       </c>
-      <c r="G17" s="115"/>
-      <c r="H17" s="68"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="103"/>
-      <c r="M17" s="103"/>
-      <c r="N17" s="103"/>
-      <c r="O17" s="103"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="104"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="68">
+        <v>4</v>
+      </c>
+      <c r="K17" s="126"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="127"/>
+      <c r="O17" s="127"/>
+      <c r="P17" s="127"/>
+      <c r="Q17" s="128"/>
     </row>
     <row r="18" spans="2:17" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="2:17" ht="25.15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4063,6 +4072,13 @@
     <row r="22" spans="2:17" ht="25.15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K13:Q14"/>
+    <mergeCell ref="K15:Q17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K2:Q5"/>
+    <mergeCell ref="K7:Q8"/>
+    <mergeCell ref="K9:Q11"/>
     <mergeCell ref="K1:Q1"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F17:G17"/>
@@ -4077,15 +4093,8 @@
     <mergeCell ref="C13:H13"/>
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="K2:Q6"/>
-    <mergeCell ref="K8:Q9"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="K10:Q11"/>
-    <mergeCell ref="K13:Q14"/>
-    <mergeCell ref="K15:Q17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>